<commit_message>
parallel exec - anu
</commit_message>
<xml_diff>
--- a/Features/CustomerDetails.xlsx
+++ b/Features/CustomerDetails.xlsx
@@ -31,16 +31,16 @@
     <t xml:space="preserve">Password</t>
   </si>
   <si>
-    <t xml:space="preserve">Gomathi Karthikeyan</t>
+    <t xml:space="preserve">Anubhooti Tyagi</t>
   </si>
   <si>
-    <t xml:space="preserve">Gomathi@123</t>
+    <t xml:space="preserve">Anu123456!</t>
   </si>
   <si>
-    <t xml:space="preserve">Karthik Kumar</t>
+    <t xml:space="preserve">Rahul Tyagi</t>
   </si>
   <si>
-    <t xml:space="preserve">Karthik@123</t>
+    <t xml:space="preserve">Rah123456!</t>
   </si>
 </sst>
 </file>
@@ -50,7 +50,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -71,20 +71,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF111111"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF1C1C1C"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -129,16 +115,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -151,66 +133,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF111111"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF1C1C1C"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -219,16 +141,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.07"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -247,7 +168,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>8939364101</v>
+        <v>9734567899</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>4</v>
@@ -258,30 +179,13 @@
         <v>5</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>9840819335</v>
+        <v>9734567889</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="Gomathi@123"/>
-    <hyperlink ref="C3" r:id="rId2" display="Karthik@123"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>